<commit_message>
extraigo y empiezo a comparar
</commit_message>
<xml_diff>
--- a/examenes finales.xlsx
+++ b/examenes finales.xlsx
@@ -13,6 +13,32 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>ingenieria electrica industrial y automatica</t>
+  </si>
+  <si>
+    <t>ingeniería electrica</t>
+  </si>
+  <si>
+    <t>ingeniería mécanica</t>
+  </si>
+  <si>
+    <t>ingeniería química</t>
+  </si>
+  <si>
+    <t>ingeniería diseño industrial y desarrollo del producto</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,8 +72,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,12 +383,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>42915</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>42915</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>42915</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>42916</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>42916</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>42916</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>42919</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>42920</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>42921</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>42922</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>42923</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>42926</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>42927</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>42928</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>42929</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>42930</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>42933</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>42934</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>42935</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>